<commit_message>
seed paper excel file added for testing
</commit_message>
<xml_diff>
--- a/backend/testing/seedPaper.xlsx
+++ b/backend/testing/seedPaper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\reactOffline\similarity\backend\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4CCF49-591A-4348-A58F-D27D318B8F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB1B5F0-D1AC-4547-8C64-1C7804D2CC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5430" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="AG29" sqref="AG29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>